<commit_message>
Nov 19 from local
</commit_message>
<xml_diff>
--- a/reference alleles.xlsx
+++ b/reference alleles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="12150" activeTab="1"/>
+    <workbookView windowWidth="20115" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="HLA-A" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="179">
   <si>
     <t>Allele</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>"5f1i"</t>
+  </si>
+  <si>
+    <t>wrong allele name, should be dog MHC</t>
   </si>
   <si>
     <t>A02_06</t>
@@ -556,12 +559,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -576,6 +579,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -584,62 +594,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -654,22 +611,45 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -684,9 +664,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -694,14 +681,6 @@
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -714,7 +693,38 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -771,25 +781,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,13 +877,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -819,103 +925,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -926,6 +936,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -946,24 +980,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -985,10 +1015,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1008,173 +1036,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1199,6 +1209,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1520,8 +1531,8 @@
   <sheetPr/>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1768,7 +1779,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" s="10" customFormat="1" spans="1:5">
+    <row r="16" s="10" customFormat="1" spans="1:6">
       <c r="A16" s="7" t="s">
         <v>35</v>
       </c>
@@ -1784,10 +1795,13 @@
       <c r="E16" s="10" t="s">
         <v>36</v>
       </c>
+      <c r="F16" s="18" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="17" s="10" customFormat="1" spans="1:5">
       <c r="A17" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>6</v>
@@ -1799,12 +1813,12 @@
         <v>28</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" s="10" customFormat="1" spans="1:5">
       <c r="A18" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>6</v>
@@ -1813,15 +1827,15 @@
         <v>27</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" s="10" customFormat="1" spans="1:4">
       <c r="A19" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>13</v>
@@ -1835,7 +1849,7 @@
     </row>
     <row r="20" s="10" customFormat="1" spans="1:4">
       <c r="A20" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>13</v>
@@ -1849,7 +1863,7 @@
     </row>
     <row r="21" s="10" customFormat="1" spans="1:4">
       <c r="A21" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>6</v>
@@ -1858,12 +1872,12 @@
         <v>27</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" s="10" customFormat="1" spans="1:4">
       <c r="A22" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>13</v>
@@ -1877,47 +1891,47 @@
     </row>
     <row r="23" s="10" customFormat="1" spans="1:5">
       <c r="A23" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" s="10" customFormat="1" spans="1:4">
       <c r="A25" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>16</v>
@@ -1925,13 +1939,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D26" s="14" t="s">
         <v>16</v>
@@ -1939,13 +1953,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>16</v>
@@ -1953,13 +1967,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="14" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D28" s="14" t="s">
         <v>11</v>
@@ -1967,30 +1981,30 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" s="10" customFormat="1" spans="1:4">
       <c r="A30" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>16</v>
@@ -1998,36 +2012,36 @@
     </row>
     <row r="31" s="10" customFormat="1" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2044,7 +2058,7 @@
   <sheetPr/>
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="E52" sqref="E52:E56"/>
     </sheetView>
   </sheetViews>
@@ -2057,869 +2071,869 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>122</v>
-      </c>
       <c r="E31" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="5" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>126</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="5" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="6" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="6" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="7" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="8" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:4">

</xml_diff>

<commit_message>
Feb 21 from local, add HLA-C
</commit_message>
<xml_diff>
--- a/reference alleles.xlsx
+++ b/reference alleles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20115" windowHeight="11955"/>
+    <workbookView windowWidth="17325" windowHeight="10890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HLA-A" sheetId="1" r:id="rId1"/>
@@ -560,8 +560,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -586,6 +586,110 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -602,63 +706,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -670,51 +722,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -722,13 +729,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -781,31 +781,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -817,115 +901,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -936,30 +936,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -980,10 +956,17 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -994,6 +977,36 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1015,186 +1028,173 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1531,8 +1531,8 @@
   <sheetPr/>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C1" sqref="C$1:C$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1718,16 +1718,16 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="10" t="s">
@@ -1735,30 +1735,30 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="10" t="s">
@@ -1766,30 +1766,30 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="B15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" s="10" customFormat="1" spans="1:6">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E16" s="10" t="s">
@@ -1800,16 +1800,16 @@
       </c>
     </row>
     <row r="17" s="10" customFormat="1" spans="1:5">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E17" s="10" t="s">
@@ -1817,16 +1817,16 @@
       </c>
     </row>
     <row r="18" s="10" customFormat="1" spans="1:5">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="B18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="9" t="s">
         <v>41</v>
       </c>
       <c r="E18" s="10" t="s">
@@ -1834,58 +1834,58 @@
       </c>
     </row>
     <row r="19" s="10" customFormat="1" spans="1:4">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="7" t="s">
+      <c r="B19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" s="10" customFormat="1" spans="1:4">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" s="10" customFormat="1" spans="1:4">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" s="10" customFormat="1" spans="1:4">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2011,16 +2011,16 @@
       </c>
     </row>
     <row r="31" s="10" customFormat="1" spans="1:5">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E31" s="10" t="s">
@@ -2028,16 +2028,16 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E32" s="10" t="s">
@@ -2058,8 +2058,8 @@
   <sheetPr/>
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52:E56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -2069,884 +2069,884 @@
     <col min="4" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D6" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:4">
+      <c r="A7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D10" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="B11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:4">
+      <c r="A13" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:4">
+      <c r="A16" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:4">
+      <c r="A17" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:4">
+      <c r="A18" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:5">
+      <c r="A19" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="4" t="s">
+    <row r="20" spans="1:4">
+      <c r="A20" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B20" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="B21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D21" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="5" t="s">
+    <row r="22" spans="1:4">
+      <c r="A22" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="B22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D22" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:4">
+      <c r="A23" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="B23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D23" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="B24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D24" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="5" t="s">
+      <c r="B25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="B26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D26" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:5">
+      <c r="A27" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="B27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D27" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:5">
+      <c r="A28" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="B28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D28" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="5" t="s">
+    <row r="29" spans="1:5">
+      <c r="A29" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="B29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D29" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:5">
+      <c r="A30" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D30" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="5" t="s">
+    <row r="31" spans="1:4">
+      <c r="A31" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="B31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D31" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="5" t="s">
+    <row r="32" spans="1:5">
+      <c r="A32" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="B32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D32" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="5" t="s">
+    <row r="33" spans="1:4">
+      <c r="A33" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="B33" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D33" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="5" t="s">
+    <row r="34" spans="1:5">
+      <c r="A34" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="5" t="s">
+      <c r="B34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D34" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="5" t="s">
+    <row r="35" spans="1:4">
+      <c r="A35" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="B35" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D35" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="5" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="B36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D36" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="5" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="B37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D37" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="5" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="B38" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D38" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="6" t="s">
+    <row r="39" spans="1:5">
+      <c r="A39" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="6" t="s">
+      <c r="B39" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D39" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="6" t="s">
+    <row r="40" spans="1:5">
+      <c r="A40" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="6" t="s">
+      <c r="B40" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D40" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="6" t="s">
+    <row r="41" spans="1:5">
+      <c r="A41" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="6" t="s">
+      <c r="B41" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D41" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="6" t="s">
+    <row r="42" spans="1:5">
+      <c r="A42" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="6" t="s">
+      <c r="B42" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D42" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="6" t="s">
+    <row r="43" spans="1:4">
+      <c r="A43" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="6" t="s">
+      <c r="B43" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D43" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="6" t="s">
+    <row r="44" spans="1:5">
+      <c r="A44" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="6" t="s">
+      <c r="B44" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D44" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="6" t="s">
+    <row r="45" spans="1:5">
+      <c r="A45" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="6" t="s">
+      <c r="B45" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D45" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="6" t="s">
+    <row r="46" spans="1:4">
+      <c r="A46" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="6" t="s">
+      <c r="B46" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D46" s="8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="7" t="s">
+    <row r="47" spans="1:4">
+      <c r="A47" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C46" s="7" t="s">
+      <c r="B47" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D47" s="9" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="7" t="s">
+    <row r="48" spans="1:4">
+      <c r="A48" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47" s="7" t="s">
+      <c r="B48" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D48" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="7" t="s">
+    <row r="49" spans="1:5">
+      <c r="A49" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="7" t="s">
+      <c r="B49" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D49" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="7" t="s">
+    <row r="50" spans="1:4">
+      <c r="A50" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="7" t="s">
+      <c r="B50" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D50" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="7" t="s">
+    <row r="51" spans="1:5">
+      <c r="A51" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" s="7" t="s">
+      <c r="B51" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D51" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="7" t="s">
+    <row r="52" spans="1:4">
+      <c r="A52" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="B51" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="7" t="s">
+      <c r="B52" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D52" s="9" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="8" t="s">
+    <row r="53" spans="1:5">
+      <c r="A53" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B52" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="8" t="s">
+      <c r="B53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D53" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="8" t="s">
+    <row r="54" spans="1:4">
+      <c r="A54" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C53" s="8" t="s">
+      <c r="B54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D53" s="8" t="s">
+      <c r="D54" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="8" t="s">
+    <row r="55" spans="1:4">
+      <c r="A55" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C54" s="8" t="s">
+      <c r="B55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D55" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="8" t="s">
+    <row r="56" spans="1:4">
+      <c r="A56" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C55" s="8" t="s">
+      <c r="B56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D55" s="8" t="s">
+      <c r="D56" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="8" t="s">
+    <row r="57" spans="1:5">
+      <c r="A57" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B56" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" s="8" t="s">
+      <c r="B57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D57" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E56" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="8" t="s">
+    <row r="58" spans="1:4">
+      <c r="A58" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B57" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C57" s="8" t="s">
+      <c r="B58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D57" s="8" t="s">
+      <c r="D58" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D58" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A1:D58">

</xml_diff>

<commit_message>
Feb 24 from local, rmsd for HLA-C
</commit_message>
<xml_diff>
--- a/reference alleles.xlsx
+++ b/reference alleles.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17325" windowHeight="10890" activeTab="1"/>
+    <workbookView windowWidth="17325" windowHeight="10890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HLA-A" sheetId="1" r:id="rId1"/>
     <sheet name="HLA-B" sheetId="2" r:id="rId2"/>
+    <sheet name="HLA-C" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="215">
   <si>
     <t>Allele</t>
   </si>
@@ -552,6 +553,114 @@
   </si>
   <si>
     <t>B52_01</t>
+  </si>
+  <si>
+    <t>Doytchinova</t>
+  </si>
+  <si>
+    <t>C01_02</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>"5w1w","5w1v"</t>
+  </si>
+  <si>
+    <t>C05_17</t>
+  </si>
+  <si>
+    <t>"5vgd"</t>
+  </si>
+  <si>
+    <t>C03_04</t>
+  </si>
+  <si>
+    <t>"1efx"</t>
+  </si>
+  <si>
+    <t>C07_56</t>
+  </si>
+  <si>
+    <t>"5vge"</t>
+  </si>
+  <si>
+    <t>C07_02</t>
+  </si>
+  <si>
+    <t>C08_01</t>
+  </si>
+  <si>
+    <t>"4nt6","6jtn","6jtp"</t>
+  </si>
+  <si>
+    <t>C12_02</t>
+  </si>
+  <si>
+    <t>C14_02</t>
+  </si>
+  <si>
+    <t>C16_01</t>
+  </si>
+  <si>
+    <t>C16_04</t>
+  </si>
+  <si>
+    <t>"5xos","5xot"</t>
+  </si>
+  <si>
+    <t>C02_02</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C03_07</t>
+  </si>
+  <si>
+    <t>C03_15</t>
+  </si>
+  <si>
+    <t>C04_01</t>
+  </si>
+  <si>
+    <t>"1qqd","1im9"</t>
+  </si>
+  <si>
+    <t>C05_01</t>
+  </si>
+  <si>
+    <t>"6jto"</t>
+  </si>
+  <si>
+    <t>C06_02</t>
+  </si>
+  <si>
+    <t>"5xs3","5w6a","5w69"</t>
+  </si>
+  <si>
+    <t>C07_07</t>
+  </si>
+  <si>
+    <t>C12_04</t>
+  </si>
+  <si>
+    <t>C12_05</t>
+  </si>
+  <si>
+    <t>C15_10</t>
+  </si>
+  <si>
+    <t>"6joz","6jp3","5t6x","5t6y","6pbh","5t6w","5t6z","5t70","6id4","5wjn","5v5m","5wjl","6mpp","5wkf","5wkh"</t>
+  </si>
+  <si>
+    <t>C16_02</t>
+  </si>
+  <si>
+    <t>C17_01</t>
+  </si>
+  <si>
+    <t>C18_01</t>
   </si>
 </sst>
 </file>
@@ -559,15 +668,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -586,8 +701,123 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -608,123 +838,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -739,13 +854,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -781,13 +896,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -799,73 +950,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -883,7 +974,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -895,37 +992,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -939,59 +1054,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1036,162 +1103,222 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -1200,16 +1327,16 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1531,516 +1658,516 @@
   <sheetPr/>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="14.44" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="16384" width="9" style="10"/>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="2" width="14.44" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9" style="5"/>
+    <col min="5" max="16384" width="9" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" s="10" customFormat="1" spans="1:12">
-      <c r="A2" s="11" t="s">
+    <row r="2" s="14" customFormat="1" spans="1:12">
+      <c r="A2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="16"/>
-    </row>
-    <row r="3" s="10" customFormat="1" spans="1:4">
-      <c r="A3" s="12" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="20"/>
+    </row>
+    <row r="3" s="14" customFormat="1" spans="1:4">
+      <c r="A3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" s="10" customFormat="1" spans="1:4">
-      <c r="A4" s="12" t="s">
+    <row r="4" s="14" customFormat="1" spans="1:4">
+      <c r="A4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" s="10" customFormat="1" spans="1:4">
-      <c r="A5" s="12" t="s">
+    <row r="5" s="14" customFormat="1" spans="1:4">
+      <c r="A5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" s="10" customFormat="1" spans="1:4">
-      <c r="A6" s="12" t="s">
+    <row r="6" s="14" customFormat="1" spans="1:4">
+      <c r="A6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" s="10" customFormat="1" spans="1:5">
-      <c r="A7" s="12" t="s">
+    <row r="7" s="14" customFormat="1" spans="1:5">
+      <c r="A7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" s="10" customFormat="1" spans="1:4">
-      <c r="A8" s="12" t="s">
+    <row r="8" s="14" customFormat="1" spans="1:4">
+      <c r="A8" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" s="10" customFormat="1" spans="1:4">
-      <c r="A9" s="12" t="s">
+    <row r="9" s="14" customFormat="1" spans="1:4">
+      <c r="A9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" s="10" customFormat="1" spans="1:5">
-      <c r="A10" s="12" t="s">
+    <row r="10" s="14" customFormat="1" spans="1:5">
+      <c r="A10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" s="10" customFormat="1" spans="1:4">
-      <c r="A11" s="12" t="s">
+    <row r="11" s="14" customFormat="1" spans="1:4">
+      <c r="A11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="B12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="14" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="9" t="s">
+      <c r="B13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" s="10" customFormat="1" spans="1:6">
-      <c r="A16" s="9" t="s">
+    <row r="16" s="14" customFormat="1" spans="1:6">
+      <c r="A16" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="B16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" s="10" customFormat="1" spans="1:5">
-      <c r="A17" s="9" t="s">
+    <row r="17" s="14" customFormat="1" spans="1:5">
+      <c r="A17" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="B17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" s="10" customFormat="1" spans="1:5">
-      <c r="A18" s="9" t="s">
+    <row r="18" s="14" customFormat="1" spans="1:5">
+      <c r="A18" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" s="10" customFormat="1" spans="1:4">
-      <c r="A19" s="9" t="s">
+    <row r="19" s="14" customFormat="1" spans="1:4">
+      <c r="A19" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="9" t="s">
+      <c r="B19" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" s="10" customFormat="1" spans="1:4">
-      <c r="A20" s="9" t="s">
+    <row r="20" s="14" customFormat="1" spans="1:4">
+      <c r="A20" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="9" t="s">
+      <c r="B20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" s="10" customFormat="1" spans="1:4">
-      <c r="A21" s="9" t="s">
+    <row r="21" s="14" customFormat="1" spans="1:4">
+      <c r="A21" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="9" t="s">
+      <c r="B21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" s="10" customFormat="1" spans="1:4">
-      <c r="A22" s="9" t="s">
+    <row r="22" s="14" customFormat="1" spans="1:4">
+      <c r="A22" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="9" t="s">
+      <c r="B22" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" s="10" customFormat="1" spans="1:5">
-      <c r="A23" s="13" t="s">
+    <row r="23" s="14" customFormat="1" spans="1:5">
+      <c r="A23" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="13" t="s">
+      <c r="B24" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" s="10" customFormat="1" spans="1:4">
-      <c r="A25" s="13" t="s">
+    <row r="25" s="14" customFormat="1" spans="1:4">
+      <c r="A25" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="13" t="s">
+      <c r="B25" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="17" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="14" t="s">
+      <c r="B26" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="18" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="14" t="s">
+      <c r="B28" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="14" t="s">
+      <c r="B29" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" s="10" customFormat="1" spans="1:4">
-      <c r="A30" s="13" t="s">
+    <row r="30" s="14" customFormat="1" spans="1:4">
+      <c r="A30" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="13" t="s">
+      <c r="B30" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="31" s="10" customFormat="1" spans="1:5">
-      <c r="A31" s="4" t="s">
+    <row r="31" s="14" customFormat="1" spans="1:5">
+      <c r="A31" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B31" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="4" t="s">
+      <c r="B32" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="14" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2058,893 +2185,893 @@
   <sheetPr/>
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="3" width="17.8866666666667" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" style="5"/>
+    <col min="2" max="3" width="17.8866666666667" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="B13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="8" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="6" t="s">
+      <c r="B20" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B22" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="B23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="7" t="s">
+      <c r="B24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="7" t="s">
+      <c r="B25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="B26" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="11" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="B27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="B28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" s="5" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="7" t="s">
+      <c r="B29" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="5" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="7" t="s">
+      <c r="B30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" s="5" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="7" t="s">
+      <c r="B31" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="11" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="7" t="s">
+      <c r="B32" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="B33" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="11" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="7" t="s">
+      <c r="B34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="7" t="s">
+      <c r="B35" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="11" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="7" t="s">
+      <c r="B36" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="11" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="7" t="s">
+      <c r="B37" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="11" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="B38" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="7" t="s">
+      <c r="B38" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="8" t="s">
+      <c r="B39" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="5" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" s="8" t="s">
+      <c r="B40" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="5" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="8" t="s">
+      <c r="B41" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="5" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="8" t="s">
+      <c r="B42" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" s="8" t="s">
+      <c r="B43" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="12" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="8" t="s">
+      <c r="B44" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="B45" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="8" t="s">
+      <c r="B45" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" s="5" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="B46" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="8" t="s">
+      <c r="B46" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="12" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="B47" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47" s="9" t="s">
+      <c r="B47" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="13" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B48" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="9" t="s">
+      <c r="B48" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="D48" s="13" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="9" t="s">
+      <c r="B49" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D49" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" s="5" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C50" s="9" t="s">
+      <c r="B50" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D50" s="13" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="B51" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="9" t="s">
+      <c r="B51" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="5" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B52" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="9" t="s">
+      <c r="B52" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D52" s="13" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="B53" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E53" s="5" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C54" s="2" t="s">
+      <c r="B54" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="B55" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="B56" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="6" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C57" s="2" t="s">
+      <c r="B57" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="D57" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" s="5" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="B58" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="6" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2955,4 +3082,234 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" t="s">
+        <v>183</v>
+      </c>
+      <c r="F2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>